<commit_message>
Code Modification To be done
</commit_message>
<xml_diff>
--- a/Hub/src/com/hub/TestData/Login Data.xlsx
+++ b/Hub/src/com/hub/TestData/Login Data.xlsx
@@ -21,14 +21,14 @@
     <t>mycallcenter2</t>
   </si>
   <si>
-    <t>Samsung888@</t>
+    <t>Trd@sm21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,10 +43,19 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,15 +90,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,7 +403,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,8 +421,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>